<commit_message>
long text bug fix
</commit_message>
<xml_diff>
--- a/Resource/All Noun.xlsx
+++ b/Resource/All Noun.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samsul Karim\Desktop\Analization folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a48a91bd88510514/Documents/UiPath/Noun Word Category Collector/Resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A336F5C-8F3E-4765-B852-53C7F94C2F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{9A336F5C-8F3E-4765-B852-53C7F94C2F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B60B8F79-58A6-4300-8591-15BCCC5250DB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="2751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="2754">
   <si>
     <t>Spanish</t>
   </si>
@@ -40,6 +40,12 @@
     <t>dentist</t>
   </si>
   <si>
+    <t>chaval</t>
+  </si>
+  <si>
+    <t>kid</t>
+  </si>
+  <si>
     <t>campesino</t>
   </si>
   <si>
@@ -139,12 +145,6 @@
     <t>swine</t>
   </si>
   <si>
-    <t>chaval</t>
-  </si>
-  <si>
-    <t>kid</t>
-  </si>
-  <si>
     <t>bailarín</t>
   </si>
   <si>
@@ -8276,6 +8276,15 @@
   </si>
   <si>
     <t>sir</t>
+  </si>
+  <si>
+    <t>1. (profession)</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>1. (fine arts)</t>
   </si>
   <si>
     <t>(profession)</t>
@@ -8600,7 +8609,7 @@
   <dimension ref="A1:B1437"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1 B1"/>
+      <selection activeCell="A3" sqref="A3 A3 A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8734,12 +8743,12 @@
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>32</v>
@@ -9206,7 +9215,7 @@
         <v>146</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -9526,7 +9535,7 @@
         <v>222</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -9646,7 +9655,7 @@
         <v>250</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -12278,7 +12287,7 @@
         <v>886</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.3">
@@ -20115,12 +20124,14 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A19" sqref="A19 A19 A19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -20142,7 +20153,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2750</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -20153,7 +20164,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2750</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -20164,7 +20175,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2750</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -20175,161 +20186,161 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2750</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -20340,7 +20351,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -20351,7 +20362,7 @@
         <v>42</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -20362,7 +20373,7 @@
         <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -20373,7 +20384,7 @@
         <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -20384,7 +20395,7 @@
         <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -20395,7 +20406,7 @@
         <v>50</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -20406,7 +20417,7 @@
         <v>52</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -20417,7 +20428,7 @@
         <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -20428,7 +20439,7 @@
         <v>56</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -20439,7 +20450,7 @@
         <v>58</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -20450,7 +20461,7 @@
         <v>60</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -20461,7 +20472,7 @@
         <v>62</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -20472,7 +20483,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -20483,7 +20494,7 @@
         <v>66</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>2750</v>
+        <v>2753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>